<commit_message>
Ajuste de la actualizacion de ingresos de datos
</commit_message>
<xml_diff>
--- a/Formato.xlsx
+++ b/Formato.xlsx
@@ -646,37 +646,37 @@
       <c r="D3" s="12" t="n"/>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>16/10/2024</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="K3" s="2" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="L3" s="6" t="inlineStr">

</xml_diff>

<commit_message>
DIAS Y MULTIPLE INGRESO
</commit_message>
<xml_diff>
--- a/Formato.xlsx
+++ b/Formato.xlsx
@@ -634,37 +634,37 @@
       <c r="D3" s="8" t="n"/>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="K3" s="2" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>27/10/2024</t>
         </is>
       </c>
       <c r="L3" s="5" t="inlineStr">

</xml_diff>